<commit_message>
Change semi-urgent default to 90 days (v0.1.35)
</commit_message>
<xml_diff>
--- a/examples/reports/Ad_med_2P.xlsx
+++ b/examples/reports/Ad_med_2P.xlsx
@@ -155,6 +155,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>21</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11430000" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>

</xml_diff>